<commit_message>
added MSXIV logo and labeled term res and cap. Changed setttings on output files and finalized panel layout
</commit_message>
<xml_diff>
--- a/MSXII_ControllerBoard/Project Outputs for Controller-Board/Controller_Board_Pick_&_Place/Controller_Board_7.0_Panel.xlsx
+++ b/MSXII_ControllerBoard/Project Outputs for Controller-Board/Controller_Board_Pick_&_Place/Controller_Board_7.0_Panel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aashmika Mali\Documents\First Year\Midnight Sun\hardware\MSXII_ControllerBoard\Project Outputs for Controller-Board\Controller_Board_Pick_&amp;_Place\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{520D0414-F2A6-4D14-AF76-DBBEF54A2F9C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BB6328E6-1C7A-4A5B-A441-1991C8936EC3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3804" yWindow="2688" windowWidth="16440" windowHeight="9420" xr2:uid="{CF872C5E-8FCA-4554-88C3-C3BDAFA3016E}"/>
+    <workbookView xWindow="3804" yWindow="2688" windowWidth="16440" windowHeight="9420" xr2:uid="{D0F0AD31-13D6-493E-95B4-1663326D1F16}"/>
   </bookViews>
   <sheets>
     <sheet name="Controller_Board_7.0_Panel" sheetId="1" r:id="rId1"/>
@@ -442,7 +442,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6500E5E1-C468-4F77-A412-2D7CCFDD4F71}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2E7807A-EEFF-4F5D-9E98-02E1766366C6}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>

</xml_diff>

<commit_message>
fixed the silksreen on the termination resistors
</commit_message>
<xml_diff>
--- a/MSXII_ControllerBoard/Project Outputs for Controller-Board/Controller_Board_Pick_&_Place/Controller_Board_7.0_Panel.xlsx
+++ b/MSXII_ControllerBoard/Project Outputs for Controller-Board/Controller_Board_Pick_&_Place/Controller_Board_7.0_Panel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aashmika Mali\Documents\First Year\Midnight Sun\hardware\MSXII_ControllerBoard\Project Outputs for Controller-Board\Controller_Board_Pick_&amp;_Place\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BB6328E6-1C7A-4A5B-A441-1991C8936EC3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FE959D2B-107E-4648-9924-1148A3F8EE6D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3804" yWindow="2688" windowWidth="16440" windowHeight="9420" xr2:uid="{D0F0AD31-13D6-493E-95B4-1663326D1F16}"/>
+    <workbookView xWindow="3804" yWindow="2688" windowWidth="16440" windowHeight="9420" xr2:uid="{5A2502A7-109E-46CB-8D4B-B724806A2074}"/>
   </bookViews>
   <sheets>
     <sheet name="Controller_Board_7.0_Panel" sheetId="1" r:id="rId1"/>
@@ -442,7 +442,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2E7807A-EEFF-4F5D-9E98-02E1766366C6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B03A66B-C28C-4067-84C1-BCA4A324B0DC}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>

</xml_diff>